<commit_message>
Add graphics and stub discussion
Graphics for charts and schematics added.
Format recorded measurements into table in report.
Prompts from lab manual added to Discussion.
</commit_message>
<xml_diff>
--- a/lab01/data/measurements.xlsx
+++ b/lab01/data/measurements.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/code/latex/elec300/lab01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/code/latex/elec300/lab01/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1.2" sheetId="1" r:id="rId1"/>
-    <sheet name="2.1" sheetId="3" r:id="rId2"/>
+    <sheet name="2.1 original" sheetId="3" r:id="rId2"/>
+    <sheet name="2.1 reformatted" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -25,15 +26,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>V_i</t>
   </si>
   <si>
-    <t>V_o</t>
+    <t>I_out</t>
   </si>
   <si>
-    <t>I_out</t>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>Vo</t>
+  </si>
+  <si>
+    <t>Io</t>
   </si>
 </sst>
 </file>
@@ -92,16 +99,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -214,6 +250,93 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF5B9BD5"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF5B9BD5"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF5B9BD5"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF5B9BD5"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -251,6 +374,17 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -322,6 +456,46 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -346,8 +520,640 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1.2'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1.2'!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>-6.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1.2'!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>-8.467</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8.468</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-8.007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-6.005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.0014</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0036</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.01</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.011</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.06</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1.2'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linear</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1.2'!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>-6.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1.2'!$C$2:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>-12.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-6.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2027094304"/>
+        <c:axId val="-2060313792"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2027094304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="7.0"/>
+          <c:min val="-7.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t>Vi (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2060313792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1.0"/>
+        <c:minorUnit val="1.0"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2060313792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="14.0"/>
+          <c:min val="-14.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t>Vo (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2027094304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2.0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.577816349384099"/>
+          <c:y val="0.15884343725327"/>
+          <c:w val="0.0839977603583427"/>
+          <c:h val="0.109756524336897"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -388,11 +1194,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1.2'!$B$1</c:f>
+              <c:f>'2.1 original'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>V_o</c:v>
+                  <c:v>I_out</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -423,96 +1229,120 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1.2'!$A$2:$A$14</c:f>
+              <c:f>'2.1 original'!$A$2:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
+                  <c:v>-8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>-6.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>-5.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>-4.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>-3.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>-2.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>-1.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>0.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>1.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>3.0</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>5.0</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1.2'!$B$2:$B$14</c:f>
+              <c:f>'2.1 original'!$B$2:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>-8.467</c:v>
+                  <c:v>-5.405</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-8.468</c:v>
+                  <c:v>-5.076</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-8.007</c:v>
+                  <c:v>-4.747</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-6.005</c:v>
+                  <c:v>-4.418</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.003</c:v>
+                  <c:v>-4.056</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.0014</c:v>
+                  <c:v>-3.043</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.001</c:v>
+                  <c:v>-2.028</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0036</c:v>
+                  <c:v>-1.014</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.007</c:v>
+                  <c:v>-0.001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.01</c:v>
+                  <c:v>1.104</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.011</c:v>
+                  <c:v>2.028</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.06</c:v>
+                  <c:v>3.042</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.06</c:v>
+                  <c:v>4.056</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.638</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.965</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.293</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -527,11 +1357,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2102545360"/>
-        <c:axId val="-2102483072"/>
+        <c:axId val="-2004503760"/>
+        <c:axId val="-2004026432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2102545360"/>
+        <c:axId val="-2004503760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -588,12 +1418,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2102483072"/>
+        <c:crossAx val="-2004026432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2102483072"/>
+        <c:axId val="-2004026432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -650,7 +1480,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2102545360"/>
+        <c:crossAx val="-2004503760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -699,7 +1529,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-CA"/>
@@ -713,38 +1543,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -755,11 +1554,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2.1'!$B$1</c:f>
+              <c:f>'2.1 reformatted'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>I_out</c:v>
+                  <c:v>Io</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -790,7 +1589,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'2.1'!$A$2:$A$18</c:f>
+              <c:f>'2.1 reformatted'!$A$2:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -850,7 +1649,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'2.1'!$B$2:$B$18</c:f>
+              <c:f>'2.1 reformatted'!$B$2:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -904,6 +1703,167 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>5.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2.1 reformatted'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linear</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'2.1 reformatted'!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>-8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-6.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'2.1 reformatted'!$C$2:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>-8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-6.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -918,13 +1878,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2080632288"/>
-        <c:axId val="-2080574112"/>
+        <c:axId val="2092126768"/>
+        <c:axId val="-2004782512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2080632288"/>
+        <c:axId val="2092126768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10.0"/>
+          <c:min val="-10.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -942,6 +1904,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t>Vi (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -964,7 +1982,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -979,14 +1997,18 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080574112"/>
+        <c:crossAx val="-2004782512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1.0"/>
+        <c:minorUnit val="1.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2080574112"/>
+        <c:axId val="-2004782512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10.0"/>
+          <c:min val="-10.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1004,6 +2026,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t>Io (mA)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1026,7 +2104,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1041,9 +2119,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080632288"/>
+        <c:crossAx val="2092126768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1053,6 +2132,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.592374020156775"/>
+          <c:y val="0.148003328852186"/>
+          <c:w val="0.0839977603583427"/>
+          <c:h val="0.109756524336897"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1091,13 +2211,10 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
   <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1170,6 +2287,43 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2202,20 +3356,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2274,23 +3944,77 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="DC_Sweep" displayName="DC_Sweep" ref="A1:B14" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6" tableBorderDxfId="9">
-  <autoFilter ref="A1:B14"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="V_i" dataDxfId="8"/>
-    <tableColumn id="2" name="V_o" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="DC_Sweep" displayName="DC_Sweep" ref="A1:C14" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="14">
+  <autoFilter ref="A1:C14"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="V_i" dataDxfId="13"/>
+    <tableColumn id="2" name="Vo" dataDxfId="12"/>
+    <tableColumn id="3" name="Linear" dataDxfId="11">
+      <calculatedColumnFormula>$A2 * 2</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Sweep2" displayName="Sweep2" ref="A1:B18" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Sweep2" displayName="Sweep2" ref="A1:B18" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A1:B18"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="V_i" dataDxfId="1"/>
-    <tableColumn id="2" name="I_out" dataDxfId="0"/>
+    <tableColumn id="1" name="V_i" dataDxfId="7"/>
+    <tableColumn id="2" name="I_out" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="DC_Sweep2" displayName="DC_Sweep2" ref="A1:C18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:C18"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="V_i" dataDxfId="2"/>
+    <tableColumn id="2" name="Io" dataDxfId="1"/>
+    <tableColumn id="3" name="Linear" dataDxfId="0">
+      <calculatedColumnFormula>$A2</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2559,124 +4283,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>-6</v>
       </c>
       <c r="B2" s="2">
         <v>-8.4670000000000005</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="3">
+        <f t="shared" ref="C2:C14" si="0">$A2 * 2</f>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>-5</v>
       </c>
       <c r="B3" s="2">
         <v>-8.468</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="3">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>-4</v>
       </c>
       <c r="B4" s="2">
         <v>-8.0069999999999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="3">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>-3</v>
       </c>
       <c r="B5" s="2">
         <v>-6.0049999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>-2</v>
       </c>
       <c r="B6" s="2">
         <v>-4.0030000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>-1</v>
       </c>
       <c r="B7" s="2">
         <v>-2.0013999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>0</v>
       </c>
       <c r="B8" s="2">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>1</v>
       </c>
       <c r="B9" s="2">
         <v>2.0036</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2</v>
       </c>
       <c r="B10" s="2">
         <v>4.0069999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>3</v>
       </c>
       <c r="B11" s="2">
         <v>6.01</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>4</v>
       </c>
       <c r="B12" s="2">
         <v>8.0109999999999992</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>5</v>
       </c>
       <c r="B13" s="2">
         <v>9.06</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>6</v>
       </c>
       <c r="B14" s="2">
         <v>9.06</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2693,7 +4472,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B18" sqref="B2:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2703,7 +4482,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2840,6 +4619,240 @@
       </c>
       <c r="B18" s="2">
         <v>5.62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>-8</v>
+      </c>
+      <c r="B2" s="3">
+        <v>-5.4050000000000002</v>
+      </c>
+      <c r="C2" s="3">
+        <f t="shared" ref="C2:C18" si="0">$A2</f>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>-7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>-5.0759999999999996</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>-6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-4.7469999999999999</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>-5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-4.4180000000000001</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>-4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-4.056</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>-3</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-3.0430000000000001</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>-2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-2.028</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-1.014</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-1E-3</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.1040000000000001</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2.028</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3.0419999999999998</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4.056</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4.6379999999999999</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4.9649999999999999</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2">
+        <v>5.2930000000000001</v>
+      </c>
+      <c r="C17" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5.62</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>